<commit_message>
Massa de dados para os testes.
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
+++ b/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao_BDD\HubTalentos-Avaliacao_BDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB4F66A-7D4B-4A5D-A8A5-02E69A9819EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEF4262-57AC-4689-A7B4-644BF93A966F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
+    <workbookView xWindow="405" yWindow="390" windowWidth="14970" windowHeight="7875" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
     <t>Maria14</t>
   </si>
   <si>
-    <t>BRUNO234</t>
+    <t>Max_Steel71</t>
   </si>
 </sst>
 </file>
@@ -1201,10 +1201,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{E6835DCD-797E-423A-91F9-44A94D89F401}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{2D786DDF-5728-4B60-AD28-AF599AF8C51C}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{F17133B7-2C6B-415C-9D6B-D05BC20E0D31}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{506B5F6E-04B9-42F4-B212-FF15B9BD919A}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{506B5F6E-04B9-42F4-B212-FF15B9BD919A}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{F17133B7-2C6B-415C-9D6B-D05BC20E0D31}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{2D786DDF-5728-4B60-AD28-AF599AF8C51C}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{E6835DCD-797E-423A-91F9-44A94D89F401}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Alteração no registro do primeiro usuario para teste.
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
+++ b/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao_BDD\HubTalentos-Avaliacao_BDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEF4262-57AC-4689-A7B4-644BF93A966F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BD0583-36DE-4146-8D4C-752088DDA963}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="405" yWindow="390" windowWidth="14970" windowHeight="7875" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
@@ -472,7 +472,7 @@
     <t>Maria14</t>
   </si>
   <si>
-    <t>Max_Steel71</t>
+    <t>Max_Steel79</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Sem alterações válidas, apenas para fins de teste da implementação do report.
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
+++ b/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao_BDD\HubTalentos-Avaliacao_BDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BD0583-36DE-4146-8D4C-752088DDA963}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E81DF2B-C59B-4666-B6BC-A1AF8D8EA670}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="390" windowWidth="14970" windowHeight="7875" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
+    <workbookView xWindow="1020" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
     <t>Maria14</t>
   </si>
   <si>
-    <t>Max_Steel79</t>
+    <t>Max_Steel97</t>
   </si>
 </sst>
 </file>
@@ -1201,10 +1201,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{506B5F6E-04B9-42F4-B212-FF15B9BD919A}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{F17133B7-2C6B-415C-9D6B-D05BC20E0D31}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{2D786DDF-5728-4B60-AD28-AF599AF8C51C}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{E6835DCD-797E-423A-91F9-44A94D89F401}"/>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{E6835DCD-797E-423A-91F9-44A94D89F401}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{2D786DDF-5728-4B60-AD28-AF599AF8C51C}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{F17133B7-2C6B-415C-9D6B-D05BC20E0D31}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{506B5F6E-04B9-42F4-B212-FF15B9BD919A}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Sem alterações válidas, apenas de formatação de texto.
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
+++ b/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao_BDD\HubTalentos-Avaliacao_BDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E81DF2B-C59B-4666-B6BC-A1AF8D8EA670}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B06DB3-4E6D-42A2-BC20-ACF422CF14C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
     <t>Maria14</t>
   </si>
   <si>
-    <t>Max_Steel97</t>
+    <t>Max_Steel103</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Alterado o nome das pastas que seram destinadas
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
+++ b/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao_BDD\HubTalentos-Avaliacao_BDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B06DB3-4E6D-42A2-BC20-ACF422CF14C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594265A1-9E53-48DD-84C8-4C871E079A7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
@@ -472,7 +472,7 @@
     <t>Maria14</t>
   </si>
   <si>
-    <t>Max_Steel103</t>
+    <t>Max_Steel112</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Mudado o nome de usuário para teste.
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
+++ b/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao_BDD\HubTalentos-Avaliacao_BDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594265A1-9E53-48DD-84C8-4C871E079A7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DA682E-BADD-4B0D-B018-084B23D25172}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
@@ -472,7 +472,7 @@
     <t>Maria14</t>
   </si>
   <si>
-    <t>Max_Steel112</t>
+    <t>Max_Steel114</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Sem alterações válidas, apenas para teste
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
+++ b/HubTalentos-Avaliacao_BDD/AdvantageOnline_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Documents\Test\test2\test3\HubTalentosAvaliacao_BDD\HubTalentos-Avaliacao_BDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83926183-9F84-4333-B358-9CEB4802AE69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB9A7EC-C816-425A-BA94-B790B7A1A40D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
@@ -472,7 +472,7 @@
     <t>Maria17</t>
   </si>
   <si>
-    <t>Max_Steel126</t>
+    <t>Max_Steel127</t>
   </si>
 </sst>
 </file>

</xml_diff>